<commit_message>
Corrected errors found in output
</commit_message>
<xml_diff>
--- a/aci-fabric-deploy-Input-Spreadsheet.xlsx
+++ b/aci-fabric-deploy-Input-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D03D38-EB82-4944-90E1-90E465C31E29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19403AC3-7ED5-4036-8822-6EFA92819F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1983,6 +1983,102 @@
     <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1995,15 +2091,6 @@
     <xf numFmtId="1" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2013,15 +2100,6 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2029,84 +2107,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2469,7 +2469,7 @@
   <dimension ref="A1:P133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,21 +2494,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2549,44 +2549,44 @@
       <c r="M3" s="13"/>
     </row>
     <row r="5" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:16" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="40" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="48"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
     </row>
     <row r="7" spans="1:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -2628,17 +2628,17 @@
       <c r="M7" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="N7" s="43" t="s">
+      <c r="N7" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="45"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="35"/>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="27" t="s">
         <v>208</v>
       </c>
       <c r="C8" s="14">
@@ -2668,47 +2668,47 @@
       <c r="K8" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="L8" s="60" t="s">
+      <c r="L8" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="M8" s="60"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="36"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="38"/>
     </row>
     <row r="10" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
     </row>
     <row r="11" spans="1:16" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
@@ -2754,13 +2754,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D13" s="14">
-        <v>201</v>
+        <v>101</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>7</v>
@@ -2769,19 +2769,19 @@
         <v>1</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>91</v>
+        <v>13</v>
+      </c>
+      <c r="H13" s="14">
+        <v>9508</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="J13" s="13" t="s">
         <v>189</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="L13" s="13" t="s">
         <v>191</v>
@@ -2793,13 +2793,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D14" s="12">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>7</v>
@@ -2814,13 +2814,13 @@
         <v>91</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>189</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>191</v>
@@ -2832,13 +2832,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="14">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>7</v>
@@ -2847,19 +2847,19 @@
         <v>1</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="14">
-        <v>9508</v>
+        <v>8</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>189</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L15" s="13" t="s">
         <v>191</v>
@@ -3032,38 +3032,38 @@
       <c r="M26" s="11"/>
     </row>
     <row r="28" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="39" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
     </row>
     <row r="29" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="50"/>
-      <c r="B29" s="51" t="s">
+      <c r="A29" s="21"/>
+      <c r="B29" s="41" t="s">
         <v>244</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
     </row>
     <row r="30" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
@@ -3206,38 +3206,38 @@
       <c r="M37" s="13"/>
     </row>
     <row r="39" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39"/>
     </row>
     <row r="40" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="53"/>
-      <c r="B40" s="54" t="s">
+      <c r="A40" s="23"/>
+      <c r="B40" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="54"/>
-      <c r="J40" s="54"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="54"/>
-      <c r="M40" s="54"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
     </row>
     <row r="41" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
@@ -3400,21 +3400,21 @@
       <c r="M48" s="13"/>
     </row>
     <row r="50" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
-      <c r="G50" s="30"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="30"/>
-      <c r="L50" s="30"/>
-      <c r="M50" s="30"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="39"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="39"/>
     </row>
     <row r="51" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
@@ -3455,38 +3455,38 @@
       <c r="M52" s="13"/>
     </row>
     <row r="54" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="30" t="s">
+      <c r="A54" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
-      <c r="L54" s="30"/>
-      <c r="M54" s="30"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="39"/>
+      <c r="L54" s="39"/>
+      <c r="M54" s="39"/>
     </row>
     <row r="55" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="53"/>
-      <c r="B55" s="54" t="s">
+      <c r="A55" s="23"/>
+      <c r="B55" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="54"/>
-      <c r="F55" s="54"/>
-      <c r="G55" s="54"/>
-      <c r="H55" s="54"/>
-      <c r="I55" s="54"/>
-      <c r="J55" s="54"/>
-      <c r="K55" s="54"/>
-      <c r="L55" s="54"/>
-      <c r="M55" s="54"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="29"/>
+      <c r="L55" s="29"/>
+      <c r="M55" s="29"/>
     </row>
     <row r="56" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
@@ -3546,21 +3546,21 @@
       <c r="M58" s="11"/>
     </row>
     <row r="60" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="30" t="s">
+      <c r="A60" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="30"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="30"/>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
-      <c r="L60" s="30"/>
-      <c r="M60" s="30"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="39"/>
     </row>
     <row r="61" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
@@ -3601,38 +3601,38 @@
       <c r="M62" s="13"/>
     </row>
     <row r="64" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="30" t="s">
+      <c r="A64" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="30"/>
-      <c r="K64" s="30"/>
-      <c r="L64" s="30"/>
-      <c r="M64" s="30"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
+      <c r="I64" s="39"/>
+      <c r="J64" s="39"/>
+      <c r="K64" s="39"/>
+      <c r="L64" s="39"/>
+      <c r="M64" s="39"/>
     </row>
     <row r="65" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="53"/>
-      <c r="B65" s="54" t="s">
+      <c r="A65" s="23"/>
+      <c r="B65" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="C65" s="54"/>
-      <c r="D65" s="54"/>
-      <c r="E65" s="54"/>
-      <c r="F65" s="54"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="54"/>
-      <c r="J65" s="54"/>
-      <c r="K65" s="54"/>
-      <c r="L65" s="54"/>
-      <c r="M65" s="54"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
+      <c r="J65" s="29"/>
+      <c r="K65" s="29"/>
+      <c r="L65" s="29"/>
+      <c r="M65" s="29"/>
     </row>
     <row r="66" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
@@ -3698,44 +3698,44 @@
       <c r="M68" s="11"/>
     </row>
     <row r="70" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="40" t="s">
+      <c r="A70" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="40"/>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="40"/>
-      <c r="F70" s="40"/>
-      <c r="G70" s="40"/>
-      <c r="H70" s="40"/>
-      <c r="I70" s="40"/>
-      <c r="J70" s="40"/>
-      <c r="K70" s="40"/>
-      <c r="L70" s="40"/>
-      <c r="M70" s="40"/>
-      <c r="N70" s="55"/>
-      <c r="O70" s="55"/>
-      <c r="P70" s="55"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="31"/>
+      <c r="H70" s="31"/>
+      <c r="I70" s="31"/>
+      <c r="J70" s="31"/>
+      <c r="K70" s="31"/>
+      <c r="L70" s="31"/>
+      <c r="M70" s="31"/>
+      <c r="N70" s="24"/>
+      <c r="O70" s="24"/>
+      <c r="P70" s="24"/>
     </row>
     <row r="71" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="56"/>
-      <c r="B71" s="57" t="s">
+      <c r="A71" s="25"/>
+      <c r="B71" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="C71" s="57"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="57"/>
-      <c r="F71" s="57"/>
-      <c r="G71" s="57"/>
-      <c r="H71" s="57"/>
-      <c r="I71" s="57"/>
-      <c r="J71" s="57"/>
-      <c r="K71" s="57"/>
-      <c r="L71" s="57"/>
-      <c r="M71" s="57"/>
-      <c r="N71" s="56"/>
-      <c r="O71" s="56"/>
-      <c r="P71" s="56"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="32"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="32"/>
+      <c r="J71" s="32"/>
+      <c r="K71" s="32"/>
+      <c r="L71" s="32"/>
+      <c r="M71" s="32"/>
+      <c r="N71" s="25"/>
+      <c r="O71" s="25"/>
+      <c r="P71" s="25"/>
     </row>
     <row r="72" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
@@ -3750,18 +3750,18 @@
       <c r="D72" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E72" s="20" t="s">
+      <c r="E72" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="F72" s="21"/>
-      <c r="G72" s="20" t="s">
+      <c r="F72" s="53"/>
+      <c r="G72" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="H72" s="21"/>
-      <c r="I72" s="20" t="s">
+      <c r="H72" s="53"/>
+      <c r="I72" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="J72" s="21"/>
+      <c r="J72" s="53"/>
       <c r="K72" s="8" t="s">
         <v>134</v>
       </c>
@@ -3794,18 +3794,18 @@
       <c r="D73" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="35" t="s">
+      <c r="E73" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="F73" s="36"/>
-      <c r="G73" s="22" t="s">
+      <c r="F73" s="38"/>
+      <c r="G73" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="H73" s="23"/>
-      <c r="I73" s="22" t="s">
+      <c r="H73" s="55"/>
+      <c r="I73" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="J73" s="23"/>
+      <c r="J73" s="55"/>
       <c r="K73" s="13" t="s">
         <v>185</v>
       </c>
@@ -3827,21 +3827,21 @@
     </row>
     <row r="74" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="30"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
-      <c r="J75" s="30"/>
-      <c r="K75" s="30"/>
-      <c r="L75" s="30"/>
-      <c r="M75" s="30"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="39"/>
+      <c r="I75" s="39"/>
+      <c r="J75" s="39"/>
+      <c r="K75" s="39"/>
+      <c r="L75" s="39"/>
+      <c r="M75" s="39"/>
     </row>
     <row r="76" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
@@ -3913,34 +3913,34 @@
       <c r="M78" s="11"/>
     </row>
     <row r="80" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="30" t="s">
+      <c r="A80" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="B80" s="30"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="30"/>
-      <c r="G80" s="30"/>
-      <c r="H80" s="30"/>
-      <c r="I80" s="30"/>
-      <c r="J80" s="30"/>
-      <c r="K80" s="30"/>
-      <c r="L80" s="30"/>
-      <c r="M80" s="30"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="39"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="39"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="39"/>
+      <c r="I80" s="39"/>
+      <c r="J80" s="39"/>
+      <c r="K80" s="39"/>
+      <c r="L80" s="39"/>
+      <c r="M80" s="39"/>
     </row>
     <row r="81" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="24" t="s">
+      <c r="B81" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C81" s="26"/>
-      <c r="D81" s="24" t="s">
+      <c r="C81" s="43"/>
+      <c r="D81" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="E81" s="26"/>
+      <c r="E81" s="43"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
@@ -3954,14 +3954,14 @@
       <c r="A82" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B82" s="38" t="s">
+      <c r="B82" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="39"/>
-      <c r="D82" s="31" t="s">
+      <c r="C82" s="45"/>
+      <c r="D82" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="E82" s="32"/>
+      <c r="E82" s="50"/>
       <c r="F82" s="13"/>
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
@@ -3975,14 +3975,14 @@
       <c r="A83" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="27" t="s">
+      <c r="B83" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="C83" s="29"/>
-      <c r="D83" s="33" t="s">
+      <c r="C83" s="58"/>
+      <c r="D83" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="E83" s="34"/>
+      <c r="E83" s="60"/>
       <c r="F83" s="11"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
@@ -3993,21 +3993,21 @@
       <c r="M83" s="11"/>
     </row>
     <row r="85" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="30" t="s">
+      <c r="A85" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="B85" s="30"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="30"/>
-      <c r="F85" s="30"/>
-      <c r="G85" s="30"/>
-      <c r="H85" s="30"/>
-      <c r="I85" s="30"/>
-      <c r="J85" s="30"/>
-      <c r="K85" s="30"/>
-      <c r="L85" s="30"/>
-      <c r="M85" s="30"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="39"/>
+      <c r="F85" s="39"/>
+      <c r="G85" s="39"/>
+      <c r="H85" s="39"/>
+      <c r="I85" s="39"/>
+      <c r="J85" s="39"/>
+      <c r="K85" s="39"/>
+      <c r="L85" s="39"/>
+      <c r="M85" s="39"/>
     </row>
     <row r="86" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
@@ -4079,35 +4079,35 @@
       <c r="M88" s="11"/>
     </row>
     <row r="90" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="30" t="s">
+      <c r="A90" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="B90" s="30"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="30"/>
-      <c r="G90" s="30"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="30"/>
-      <c r="J90" s="30"/>
-      <c r="K90" s="30"/>
-      <c r="L90" s="30"/>
-      <c r="M90" s="30"/>
+      <c r="B90" s="39"/>
+      <c r="C90" s="39"/>
+      <c r="D90" s="39"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="39"/>
+      <c r="G90" s="39"/>
+      <c r="H90" s="39"/>
+      <c r="I90" s="39"/>
+      <c r="J90" s="39"/>
+      <c r="K90" s="39"/>
+      <c r="L90" s="39"/>
+      <c r="M90" s="39"/>
     </row>
     <row r="91" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="25" t="s">
+      <c r="B91" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="C91" s="25"/>
-      <c r="D91" s="24" t="s">
+      <c r="C91" s="47"/>
+      <c r="D91" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="E91" s="25"/>
-      <c r="F91" s="26"/>
+      <c r="E91" s="47"/>
+      <c r="F91" s="43"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
@@ -4120,15 +4120,15 @@
       <c r="A92" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B92" s="38" t="s">
+      <c r="B92" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C92" s="39"/>
-      <c r="D92" s="31" t="s">
+      <c r="C92" s="45"/>
+      <c r="D92" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E92" s="41"/>
-      <c r="F92" s="32"/>
+      <c r="E92" s="49"/>
+      <c r="F92" s="50"/>
       <c r="G92" s="14"/>
       <c r="H92" s="14"/>
       <c r="I92" s="13"/>
@@ -4141,38 +4141,38 @@
       <c r="B93" s="7"/>
     </row>
     <row r="94" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="30" t="s">
+      <c r="A94" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="B94" s="30"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="30"/>
-      <c r="G94" s="30"/>
-      <c r="H94" s="30"/>
-      <c r="I94" s="30"/>
-      <c r="J94" s="30"/>
-      <c r="K94" s="30"/>
-      <c r="L94" s="30"/>
-      <c r="M94" s="30"/>
+      <c r="B94" s="39"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="39"/>
+      <c r="F94" s="39"/>
+      <c r="G94" s="39"/>
+      <c r="H94" s="39"/>
+      <c r="I94" s="39"/>
+      <c r="J94" s="39"/>
+      <c r="K94" s="39"/>
+      <c r="L94" s="39"/>
+      <c r="M94" s="39"/>
     </row>
     <row r="95" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="53"/>
-      <c r="B95" s="54" t="s">
+      <c r="A95" s="23"/>
+      <c r="B95" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="C95" s="54"/>
-      <c r="D95" s="54"/>
-      <c r="E95" s="54"/>
-      <c r="F95" s="54"/>
-      <c r="G95" s="54"/>
-      <c r="H95" s="54"/>
-      <c r="I95" s="54"/>
-      <c r="J95" s="54"/>
-      <c r="K95" s="54"/>
-      <c r="L95" s="54"/>
-      <c r="M95" s="54"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="29"/>
+      <c r="G95" s="29"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="29"/>
+      <c r="J95" s="29"/>
+      <c r="K95" s="29"/>
+      <c r="L95" s="29"/>
+      <c r="M95" s="29"/>
     </row>
     <row r="96" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
@@ -4181,11 +4181,11 @@
       <c r="B96" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C96" s="24" t="s">
+      <c r="C96" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D96" s="25"/>
-      <c r="E96" s="26"/>
+      <c r="D96" s="47"/>
+      <c r="E96" s="43"/>
       <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
@@ -4199,14 +4199,14 @@
       <c r="A97" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B97" s="60" t="s">
+      <c r="B97" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C97" s="38" t="s">
+      <c r="C97" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="D97" s="42"/>
-      <c r="E97" s="39"/>
+      <c r="D97" s="51"/>
+      <c r="E97" s="45"/>
       <c r="F97" s="13"/>
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
@@ -4220,14 +4220,14 @@
       <c r="A98" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B98" s="61" t="s">
+      <c r="B98" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C98" s="27" t="s">
+      <c r="C98" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="D98" s="28"/>
-      <c r="E98" s="29"/>
+      <c r="D98" s="57"/>
+      <c r="E98" s="58"/>
       <c r="F98" s="11"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
@@ -4239,38 +4239,38 @@
     </row>
     <row r="99" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="40" t="s">
+      <c r="A100" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="B100" s="40"/>
-      <c r="C100" s="40"/>
-      <c r="D100" s="40"/>
-      <c r="E100" s="40"/>
-      <c r="F100" s="40"/>
-      <c r="G100" s="40"/>
-      <c r="H100" s="40"/>
-      <c r="I100" s="40"/>
-      <c r="J100" s="40"/>
-      <c r="K100" s="40"/>
-      <c r="L100" s="40"/>
-      <c r="M100" s="40"/>
+      <c r="B100" s="31"/>
+      <c r="C100" s="31"/>
+      <c r="D100" s="31"/>
+      <c r="E100" s="31"/>
+      <c r="F100" s="31"/>
+      <c r="G100" s="31"/>
+      <c r="H100" s="31"/>
+      <c r="I100" s="31"/>
+      <c r="J100" s="31"/>
+      <c r="K100" s="31"/>
+      <c r="L100" s="31"/>
+      <c r="M100" s="31"/>
     </row>
     <row r="101" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="53"/>
-      <c r="B101" s="54" t="s">
+      <c r="A101" s="23"/>
+      <c r="B101" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="C101" s="54"/>
-      <c r="D101" s="54"/>
-      <c r="E101" s="54"/>
-      <c r="F101" s="54"/>
-      <c r="G101" s="54"/>
-      <c r="H101" s="54"/>
-      <c r="I101" s="54"/>
-      <c r="J101" s="54"/>
-      <c r="K101" s="54"/>
-      <c r="L101" s="54"/>
-      <c r="M101" s="54"/>
+      <c r="C101" s="29"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="29"/>
+      <c r="H101" s="29"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="29"/>
+      <c r="K101" s="29"/>
+      <c r="L101" s="29"/>
+      <c r="M101" s="29"/>
     </row>
     <row r="102" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
@@ -4314,7 +4314,7 @@
       <c r="D103" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E103" s="60" t="s">
+      <c r="E103" s="27" t="s">
         <v>38</v>
       </c>
       <c r="F103" s="13" t="s">
@@ -4343,7 +4343,7 @@
       <c r="D104" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E104" s="61" t="s">
+      <c r="E104" s="28" t="s">
         <v>44</v>
       </c>
       <c r="F104" s="11" t="s">
@@ -4361,38 +4361,38 @@
     </row>
     <row r="105" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="30" t="s">
+      <c r="A106" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="B106" s="30"/>
-      <c r="C106" s="30"/>
-      <c r="D106" s="30"/>
-      <c r="E106" s="30"/>
-      <c r="F106" s="30"/>
-      <c r="G106" s="30"/>
-      <c r="H106" s="30"/>
-      <c r="I106" s="30"/>
-      <c r="J106" s="30"/>
-      <c r="K106" s="30"/>
-      <c r="L106" s="30"/>
-      <c r="M106" s="30"/>
+      <c r="B106" s="39"/>
+      <c r="C106" s="39"/>
+      <c r="D106" s="39"/>
+      <c r="E106" s="39"/>
+      <c r="F106" s="39"/>
+      <c r="G106" s="39"/>
+      <c r="H106" s="39"/>
+      <c r="I106" s="39"/>
+      <c r="J106" s="39"/>
+      <c r="K106" s="39"/>
+      <c r="L106" s="39"/>
+      <c r="M106" s="39"/>
     </row>
     <row r="107" spans="1:13" s="3" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="53"/>
-      <c r="B107" s="54" t="s">
+      <c r="A107" s="23"/>
+      <c r="B107" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="C107" s="54"/>
-      <c r="D107" s="54"/>
-      <c r="E107" s="54"/>
-      <c r="F107" s="54"/>
-      <c r="G107" s="54"/>
-      <c r="H107" s="54"/>
-      <c r="I107" s="54"/>
-      <c r="J107" s="54"/>
-      <c r="K107" s="54"/>
-      <c r="L107" s="54"/>
-      <c r="M107" s="54"/>
+      <c r="C107" s="29"/>
+      <c r="D107" s="29"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+      <c r="G107" s="29"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
+      <c r="J107" s="29"/>
+      <c r="K107" s="29"/>
+      <c r="L107" s="29"/>
+      <c r="M107" s="29"/>
     </row>
     <row r="108" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
@@ -4431,13 +4431,13 @@
       <c r="C109" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D109" s="60" t="s">
+      <c r="D109" s="27" t="s">
         <v>48</v>
       </c>
       <c r="E109" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F109" s="60" t="s">
+      <c r="F109" s="27" t="s">
         <v>48</v>
       </c>
       <c r="G109" s="14"/>
@@ -4458,13 +4458,13 @@
       <c r="C110" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D110" s="61" t="s">
+      <c r="D110" s="28" t="s">
         <v>48</v>
       </c>
       <c r="E110" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F110" s="61" t="s">
+      <c r="F110" s="28" t="s">
         <v>48</v>
       </c>
       <c r="G110" s="12"/>
@@ -4485,11 +4485,11 @@
       <c r="C111" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D111" s="60"/>
+      <c r="D111" s="27"/>
       <c r="E111" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F111" s="60" t="s">
+      <c r="F111" s="27" t="s">
         <v>48</v>
       </c>
       <c r="G111" s="14"/>
@@ -4502,21 +4502,21 @@
     </row>
     <row r="112" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="113" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="30" t="s">
+      <c r="A113" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="B113" s="30"/>
-      <c r="C113" s="30"/>
-      <c r="D113" s="30"/>
-      <c r="E113" s="30"/>
-      <c r="F113" s="30"/>
-      <c r="G113" s="30"/>
-      <c r="H113" s="30"/>
-      <c r="I113" s="30"/>
-      <c r="J113" s="30"/>
-      <c r="K113" s="30"/>
-      <c r="L113" s="30"/>
-      <c r="M113" s="30"/>
+      <c r="B113" s="39"/>
+      <c r="C113" s="39"/>
+      <c r="D113" s="39"/>
+      <c r="E113" s="39"/>
+      <c r="F113" s="39"/>
+      <c r="G113" s="39"/>
+      <c r="H113" s="39"/>
+      <c r="I113" s="39"/>
+      <c r="J113" s="39"/>
+      <c r="K113" s="39"/>
+      <c r="L113" s="39"/>
+      <c r="M113" s="39"/>
     </row>
     <row r="114" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
@@ -4590,38 +4590,38 @@
     </row>
     <row r="116" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="117" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="30" t="s">
+      <c r="A117" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="B117" s="30"/>
-      <c r="C117" s="30"/>
-      <c r="D117" s="30"/>
-      <c r="E117" s="30"/>
-      <c r="F117" s="30"/>
-      <c r="G117" s="30"/>
-      <c r="H117" s="30"/>
-      <c r="I117" s="30"/>
-      <c r="J117" s="30"/>
-      <c r="K117" s="30"/>
-      <c r="L117" s="30"/>
-      <c r="M117" s="30"/>
+      <c r="B117" s="39"/>
+      <c r="C117" s="39"/>
+      <c r="D117" s="39"/>
+      <c r="E117" s="39"/>
+      <c r="F117" s="39"/>
+      <c r="G117" s="39"/>
+      <c r="H117" s="39"/>
+      <c r="I117" s="39"/>
+      <c r="J117" s="39"/>
+      <c r="K117" s="39"/>
+      <c r="L117" s="39"/>
+      <c r="M117" s="39"/>
     </row>
     <row r="118" spans="1:13" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="58"/>
-      <c r="B118" s="59" t="s">
+      <c r="A118" s="26"/>
+      <c r="B118" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="C118" s="59"/>
-      <c r="D118" s="59"/>
-      <c r="E118" s="59"/>
-      <c r="F118" s="59"/>
-      <c r="G118" s="59"/>
-      <c r="H118" s="59"/>
-      <c r="I118" s="59"/>
-      <c r="J118" s="59"/>
-      <c r="K118" s="59"/>
-      <c r="L118" s="59"/>
-      <c r="M118" s="59"/>
+      <c r="C118" s="30"/>
+      <c r="D118" s="30"/>
+      <c r="E118" s="30"/>
+      <c r="F118" s="30"/>
+      <c r="G118" s="30"/>
+      <c r="H118" s="30"/>
+      <c r="I118" s="30"/>
+      <c r="J118" s="30"/>
+      <c r="K118" s="30"/>
+      <c r="L118" s="30"/>
+      <c r="M118" s="30"/>
     </row>
     <row r="119" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
@@ -4669,7 +4669,7 @@
       <c r="D120" s="14">
         <v>1812</v>
       </c>
-      <c r="E120" s="60" t="s">
+      <c r="E120" s="27" t="s">
         <v>67</v>
       </c>
       <c r="F120" s="13" t="s">
@@ -4702,7 +4702,7 @@
       <c r="D121" s="12">
         <v>1812</v>
       </c>
-      <c r="E121" s="61" t="s">
+      <c r="E121" s="28" t="s">
         <v>48</v>
       </c>
       <c r="F121" s="11" t="s">
@@ -4724,38 +4724,38 @@
     </row>
     <row r="122" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="123" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="30" t="s">
+      <c r="A123" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="B123" s="30"/>
-      <c r="C123" s="30"/>
-      <c r="D123" s="30"/>
-      <c r="E123" s="30"/>
-      <c r="F123" s="30"/>
-      <c r="G123" s="30"/>
-      <c r="H123" s="30"/>
-      <c r="I123" s="30"/>
-      <c r="J123" s="30"/>
-      <c r="K123" s="30"/>
-      <c r="L123" s="30"/>
-      <c r="M123" s="30"/>
+      <c r="B123" s="39"/>
+      <c r="C123" s="39"/>
+      <c r="D123" s="39"/>
+      <c r="E123" s="39"/>
+      <c r="F123" s="39"/>
+      <c r="G123" s="39"/>
+      <c r="H123" s="39"/>
+      <c r="I123" s="39"/>
+      <c r="J123" s="39"/>
+      <c r="K123" s="39"/>
+      <c r="L123" s="39"/>
+      <c r="M123" s="39"/>
     </row>
     <row r="124" spans="1:13" ht="69.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="58"/>
-      <c r="B124" s="59" t="s">
+      <c r="A124" s="26"/>
+      <c r="B124" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="C124" s="59"/>
-      <c r="D124" s="59"/>
-      <c r="E124" s="59"/>
-      <c r="F124" s="59"/>
-      <c r="G124" s="59"/>
-      <c r="H124" s="59"/>
-      <c r="I124" s="59"/>
-      <c r="J124" s="59"/>
-      <c r="K124" s="59"/>
-      <c r="L124" s="59"/>
-      <c r="M124" s="59"/>
+      <c r="C124" s="30"/>
+      <c r="D124" s="30"/>
+      <c r="E124" s="30"/>
+      <c r="F124" s="30"/>
+      <c r="G124" s="30"/>
+      <c r="H124" s="30"/>
+      <c r="I124" s="30"/>
+      <c r="J124" s="30"/>
+      <c r="K124" s="30"/>
+      <c r="L124" s="30"/>
+      <c r="M124" s="30"/>
     </row>
     <row r="125" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
@@ -4803,7 +4803,7 @@
       <c r="D126" s="14">
         <v>49</v>
       </c>
-      <c r="E126" s="60" t="s">
+      <c r="E126" s="27" t="s">
         <v>67</v>
       </c>
       <c r="F126" s="13" t="s">
@@ -4836,7 +4836,7 @@
       <c r="D127" s="12">
         <v>49</v>
       </c>
-      <c r="E127" s="61" t="s">
+      <c r="E127" s="28" t="s">
         <v>48</v>
       </c>
       <c r="F127" s="11" t="s">
@@ -4857,38 +4857,38 @@
       <c r="M127" s="11"/>
     </row>
     <row r="129" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="37" t="s">
+      <c r="A129" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="B129" s="37"/>
-      <c r="C129" s="37"/>
-      <c r="D129" s="37"/>
-      <c r="E129" s="37"/>
-      <c r="F129" s="37"/>
-      <c r="G129" s="37"/>
-      <c r="H129" s="37"/>
-      <c r="I129" s="37"/>
-      <c r="J129" s="37"/>
-      <c r="K129" s="37"/>
-      <c r="L129" s="37"/>
-      <c r="M129" s="37"/>
+      <c r="B129" s="46"/>
+      <c r="C129" s="46"/>
+      <c r="D129" s="46"/>
+      <c r="E129" s="46"/>
+      <c r="F129" s="46"/>
+      <c r="G129" s="46"/>
+      <c r="H129" s="46"/>
+      <c r="I129" s="46"/>
+      <c r="J129" s="46"/>
+      <c r="K129" s="46"/>
+      <c r="L129" s="46"/>
+      <c r="M129" s="46"/>
     </row>
     <row r="130" spans="1:13" s="3" customFormat="1" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="58"/>
-      <c r="B130" s="59" t="s">
+      <c r="A130" s="26"/>
+      <c r="B130" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="C130" s="59"/>
-      <c r="D130" s="59"/>
-      <c r="E130" s="59"/>
-      <c r="F130" s="59"/>
-      <c r="G130" s="59"/>
-      <c r="H130" s="59"/>
-      <c r="I130" s="59"/>
-      <c r="J130" s="59"/>
-      <c r="K130" s="59"/>
-      <c r="L130" s="59"/>
-      <c r="M130" s="59"/>
+      <c r="C130" s="30"/>
+      <c r="D130" s="30"/>
+      <c r="E130" s="30"/>
+      <c r="F130" s="30"/>
+      <c r="G130" s="30"/>
+      <c r="H130" s="30"/>
+      <c r="I130" s="30"/>
+      <c r="J130" s="30"/>
+      <c r="K130" s="30"/>
+      <c r="L130" s="30"/>
+      <c r="M130" s="30"/>
     </row>
     <row r="131" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
@@ -4959,51 +4959,6 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B101:M101"/>
-    <mergeCell ref="B107:M107"/>
-    <mergeCell ref="B118:M118"/>
-    <mergeCell ref="B130:M130"/>
-    <mergeCell ref="B124:M124"/>
-    <mergeCell ref="B55:M55"/>
-    <mergeCell ref="B65:M65"/>
-    <mergeCell ref="A70:M70"/>
-    <mergeCell ref="B71:M71"/>
-    <mergeCell ref="B95:M95"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A50:M50"/>
-    <mergeCell ref="A54:M54"/>
-    <mergeCell ref="A28:M28"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B40:M40"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="A123:M123"/>
-    <mergeCell ref="A94:M94"/>
-    <mergeCell ref="A64:M64"/>
-    <mergeCell ref="A60:M60"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="A113:M113"/>
-    <mergeCell ref="A117:M117"/>
-    <mergeCell ref="A129:M129"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A106:M106"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="A90:M90"/>
     <mergeCell ref="A75:M75"/>
     <mergeCell ref="A80:M80"/>
     <mergeCell ref="A85:M85"/>
@@ -5014,6 +4969,51 @@
     <mergeCell ref="D83:E83"/>
     <mergeCell ref="E72:F72"/>
     <mergeCell ref="E73:F73"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="A106:M106"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A50:M50"/>
+    <mergeCell ref="A54:M54"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B40:M40"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="B55:M55"/>
+    <mergeCell ref="B65:M65"/>
+    <mergeCell ref="A70:M70"/>
+    <mergeCell ref="B71:M71"/>
+    <mergeCell ref="B95:M95"/>
+    <mergeCell ref="A94:M94"/>
+    <mergeCell ref="A64:M64"/>
+    <mergeCell ref="A60:M60"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="A90:M90"/>
+    <mergeCell ref="B101:M101"/>
+    <mergeCell ref="B107:M107"/>
+    <mergeCell ref="B118:M118"/>
+    <mergeCell ref="B130:M130"/>
+    <mergeCell ref="B124:M124"/>
+    <mergeCell ref="A123:M123"/>
+    <mergeCell ref="A113:M113"/>
+    <mergeCell ref="A117:M117"/>
+    <mergeCell ref="A129:M129"/>
   </mergeCells>
   <dataValidations count="59">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -5022,17 +5022,17 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E26" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"unspecified,remote-leaf-wan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G26 G31:G37" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G31:G37 G13:G26" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>switch_role</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H26 H31:H37" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H37 H13:H26" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>INDIRECT(G13)</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inband VLAN" error="VLAN must be between 5 and 3097" sqref="B3" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>5</formula1>
       <formula2>3097</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="D31:E37 D13:D26 C57:C58" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="D31:E37 C57:C58 D13:D26" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>101</formula1>
       <formula2>4000</formula2>
     </dataValidation>
@@ -5049,7 +5049,7 @@
       <formula1>1</formula1>
       <formula2>4294967295</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pod ID" error="Pod Id must be between 1 and 12!" sqref="D42:D48 F13:F26 F31:F37" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pod ID" error="Pod Id must be between 1 and 12!" sqref="D42:D48 F31:F37 F13:F26" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>

</xml_diff>